<commit_message>
Changed LV data to timeseries from plot in original paper
</commit_message>
<xml_diff>
--- a/Tests/Validation/Stock/FeedLotObserved.xlsx
+++ b/Tests/Validation/Stock/FeedLotObserved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\Validation\Stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB18A09-1EAE-4344-B7C0-8615A09A086E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6A6E76-0660-478F-B17A-A3A99581C99D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29730" yWindow="3960" windowWidth="16200" windowHeight="9990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidationData" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
   <si>
     <t>SimulationName</t>
   </si>
@@ -53,9 +53,6 @@
     <t>DaysOfFeed</t>
   </si>
   <si>
-    <t>MeanDailyIntake</t>
-  </si>
-  <si>
     <t>AssumedStartDate</t>
   </si>
   <si>
@@ -69,13 +66,16 @@
   </si>
   <si>
     <t>Clock.Today</t>
+  </si>
+  <si>
+    <t>Stock.Intake.All</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,13 +89,24 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF2C2C2C"/>
+      <name val="Var(--inter)"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -114,7 +125,9 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,13 +409,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="14.86328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.19921875" bestFit="1" customWidth="1"/>
@@ -410,116 +423,346 @@
     <col min="4" max="4" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.46484375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <f>C2+D2</f>
-        <v>36736</v>
+        <v>36647</v>
       </c>
       <c r="C2" s="1">
         <v>36647</v>
       </c>
-      <c r="D2" s="2">
-        <v>89</v>
-      </c>
-      <c r="E2">
-        <v>10.7</v>
-      </c>
-      <c r="F2">
-        <v>563</v>
-      </c>
-      <c r="G2">
-        <f>E2*D2</f>
-        <v>952.3</v>
-      </c>
-      <c r="H2">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:B4" si="0">C3+D3</f>
-        <v>36763</v>
+        <f t="shared" ref="B3:B17" si="0">C3+D3</f>
+        <v>36676</v>
       </c>
       <c r="C3" s="1">
         <v>36647</v>
       </c>
-      <c r="D3" s="2">
-        <v>116</v>
-      </c>
-      <c r="E3">
-        <v>10.4</v>
-      </c>
-      <c r="F3">
-        <v>524</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G4" si="1">E3*D3</f>
-        <v>1206.4000000000001</v>
-      </c>
-      <c r="H3">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D3">
+        <v>29</v>
+      </c>
+      <c r="F3" s="2">
+        <v>318.102508178844</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <f t="shared" si="0"/>
+        <v>36697</v>
+      </c>
+      <c r="C4" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+      <c r="F4" s="2">
+        <v>367.72082878953103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" si="0"/>
+        <v>36736</v>
+      </c>
+      <c r="C5" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D5">
+        <v>89</v>
+      </c>
+      <c r="F5" s="2">
+        <v>454.96183206106798</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
+        <v>36763</v>
+      </c>
+      <c r="C6" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D6">
+        <v>116</v>
+      </c>
+      <c r="F6" s="2">
+        <v>495.85605234460098</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>36792</v>
+      </c>
+      <c r="C7" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D7">
+        <v>145</v>
+      </c>
+      <c r="F7" s="2">
+        <v>534.56924754634599</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
         <v>36810</v>
       </c>
-      <c r="C4" s="1">
-        <v>36647</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C8" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D8">
         <v>163</v>
       </c>
-      <c r="E4">
+      <c r="E8">
         <v>10.199999999999999</v>
       </c>
-      <c r="F4">
-        <v>555</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="1"/>
+      <c r="F8">
+        <v>570</v>
+      </c>
+      <c r="G8">
+        <f>D8*E8</f>
         <v>1662.6</v>
       </c>
-      <c r="H4">
+      <c r="H8">
         <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>36647</v>
+      </c>
+      <c r="C9" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>36676</v>
+      </c>
+      <c r="C10" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D10">
+        <v>29</v>
+      </c>
+      <c r="F10" s="2">
+        <v>381.35223555070797</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>36697</v>
+      </c>
+      <c r="C11" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D11">
+        <v>50</v>
+      </c>
+      <c r="F11" s="2">
+        <v>431.51581243184199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>36736</v>
+      </c>
+      <c r="C12" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D12">
+        <v>89</v>
+      </c>
+      <c r="F12" s="2">
+        <v>515.48527808069798</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>36763</v>
+      </c>
+      <c r="C13" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D13">
+        <v>116</v>
+      </c>
+      <c r="E13">
+        <v>10.4</v>
+      </c>
+      <c r="F13">
+        <v>547</v>
+      </c>
+      <c r="G13">
+        <f>D13*E13</f>
+        <v>1206.4000000000001</v>
+      </c>
+      <c r="H13">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>36647</v>
+      </c>
+      <c r="C14" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>36676</v>
+      </c>
+      <c r="C15" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D15">
+        <v>29</v>
+      </c>
+      <c r="F15" s="2">
+        <v>466.95747001090501</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>36697</v>
+      </c>
+      <c r="C16" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D16">
+        <v>50</v>
+      </c>
+      <c r="F16" s="2">
+        <v>516.57579062159198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>36736</v>
+      </c>
+      <c r="C17" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D17">
+        <v>89</v>
+      </c>
+      <c r="E17">
+        <v>10.7</v>
+      </c>
+      <c r="F17">
+        <v>588</v>
+      </c>
+      <c r="G17">
+        <f>D17*E17</f>
+        <v>952.3</v>
+      </c>
+      <c r="H17">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change to use Date instead of Clock.Today
</commit_message>
<xml_diff>
--- a/Tests/Validation/Stock/FeedLotObserved.xlsx
+++ b/Tests/Validation/Stock/FeedLotObserved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\Validation\Stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009FD540-8BB2-4892-A650-ED798BDBAFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF06820-A87A-4B61-A56C-FE216E890B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,9 +65,6 @@
     <t>LiveWtGain</t>
   </si>
   <si>
-    <t>Clock.Today</t>
-  </si>
-  <si>
     <t>Stock.Intake.All</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>Hersom2HGW</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" activeCellId="1" sqref="D2:D32 F2:F32"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -432,7 +432,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -441,7 +441,7 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
@@ -761,7 +761,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
@@ -776,7 +776,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="1">
         <f t="shared" si="0"/>
@@ -794,7 +794,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" s="1">
         <f t="shared" si="0"/>
@@ -812,7 +812,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" s="1">
         <f t="shared" si="0"/>
@@ -830,7 +830,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1">
         <f t="shared" si="0"/>
@@ -848,7 +848,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23" s="1">
         <f t="shared" si="0"/>
@@ -875,7 +875,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24" s="1">
         <f t="shared" si="0"/>
@@ -890,7 +890,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B25" s="1">
         <f t="shared" si="0"/>
@@ -908,7 +908,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B26" s="1">
         <f t="shared" si="0"/>
@@ -926,7 +926,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B27" s="1">
         <f t="shared" si="0"/>
@@ -944,7 +944,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" s="1">
         <f t="shared" si="0"/>
@@ -971,7 +971,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B29" s="1">
         <f t="shared" si="0"/>
@@ -986,7 +986,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B30" s="1">
         <f t="shared" si="0"/>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B31" s="1">
         <f t="shared" si="0"/>
@@ -1022,7 +1022,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B32" s="1">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Add Sharman test data sets
</commit_message>
<xml_diff>
--- a/Tests/Validation/Stock/FeedLotObserved.xlsx
+++ b/Tests/Validation/Stock/FeedLotObserved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\Validation\Stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF06820-A87A-4B61-A56C-FE216E890B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92B59A2-7150-4358-B974-BFFEA77EB256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38505" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidationData" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
   <si>
     <t>SimulationName</t>
   </si>
@@ -78,6 +78,30 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Sharman1CON</t>
+  </si>
+  <si>
+    <t>Sharman1CORN</t>
+  </si>
+  <si>
+    <t>Sharman1LGWP</t>
+  </si>
+  <si>
+    <t>Sharman1HGWP</t>
+  </si>
+  <si>
+    <t>Sharman2CON</t>
+  </si>
+  <si>
+    <t>Sharman2CORN</t>
+  </si>
+  <si>
+    <t>Sharman2LGWP</t>
+  </si>
+  <si>
+    <t>Sharman2HGWP</t>
   </si>
 </sst>
 </file>
@@ -409,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1047,6 +1071,230 @@
         <v>147</v>
       </c>
     </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="1">
+        <f t="shared" ref="B33:B36" si="1">C33+D33</f>
+        <v>36759</v>
+      </c>
+      <c r="C33" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D33">
+        <v>112</v>
+      </c>
+      <c r="E33">
+        <v>12.1</v>
+      </c>
+      <c r="F33" s="3">
+        <v>597</v>
+      </c>
+      <c r="G33">
+        <f>D33*E33</f>
+        <v>1355.2</v>
+      </c>
+      <c r="H33">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="1">
+        <f t="shared" si="1"/>
+        <v>36759</v>
+      </c>
+      <c r="C34" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D34">
+        <v>112</v>
+      </c>
+      <c r="E34">
+        <v>12.5</v>
+      </c>
+      <c r="F34" s="3">
+        <v>632</v>
+      </c>
+      <c r="G34">
+        <f t="shared" ref="G34:G36" si="2">D34*E34</f>
+        <v>1400</v>
+      </c>
+      <c r="H34">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="1">
+        <f t="shared" si="1"/>
+        <v>36785</v>
+      </c>
+      <c r="C35" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D35">
+        <v>138</v>
+      </c>
+      <c r="E35">
+        <v>11.8</v>
+      </c>
+      <c r="F35" s="3">
+        <v>610</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="2"/>
+        <v>1628.4</v>
+      </c>
+      <c r="H35">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="1">
+        <f t="shared" si="1"/>
+        <v>36730</v>
+      </c>
+      <c r="C36" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D36">
+        <v>83</v>
+      </c>
+      <c r="E36">
+        <v>11.2</v>
+      </c>
+      <c r="F36" s="3">
+        <v>588</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="2"/>
+        <v>929.59999999999991</v>
+      </c>
+      <c r="H36">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="1">
+        <f t="shared" ref="B37:B40" si="3">C37+D37</f>
+        <v>36759</v>
+      </c>
+      <c r="C37" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D37">
+        <v>112</v>
+      </c>
+      <c r="E37">
+        <v>11.9</v>
+      </c>
+      <c r="F37" s="3">
+        <v>617</v>
+      </c>
+      <c r="G37">
+        <f>D37*E37</f>
+        <v>1332.8</v>
+      </c>
+      <c r="H37">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="1">
+        <f t="shared" si="3"/>
+        <v>36793</v>
+      </c>
+      <c r="C38" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D38">
+        <v>146</v>
+      </c>
+      <c r="E38">
+        <v>10</v>
+      </c>
+      <c r="F38" s="3">
+        <v>590</v>
+      </c>
+      <c r="G38">
+        <f t="shared" ref="G38:G40" si="4">D38*E38</f>
+        <v>1460</v>
+      </c>
+      <c r="H38">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" s="1">
+        <f t="shared" si="3"/>
+        <v>36775</v>
+      </c>
+      <c r="C39" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D39">
+        <v>128</v>
+      </c>
+      <c r="E39">
+        <v>10</v>
+      </c>
+      <c r="F39" s="3">
+        <v>575</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="4"/>
+        <v>1280</v>
+      </c>
+      <c r="H39">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="1">
+        <f t="shared" si="3"/>
+        <v>36778</v>
+      </c>
+      <c r="C40" s="1">
+        <v>36647</v>
+      </c>
+      <c r="D40">
+        <v>131</v>
+      </c>
+      <c r="E40">
+        <v>10.5</v>
+      </c>
+      <c r="F40" s="3">
+        <v>581</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="4"/>
+        <v>1375.5</v>
+      </c>
+      <c r="H40">
+        <v>223</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes via meeting with Adam and James
</commit_message>
<xml_diff>
--- a/Tests/Validation/Stock/FeedLotObserved.xlsx
+++ b/Tests/Validation/Stock/FeedLotObserved.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\Validation\Stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB5DEC0-5601-4125-BCFF-A992F287D697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FE0081-5A91-4D5A-8BB3-D7067A9D1BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47910" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidationData" sheetId="1" r:id="rId1"/>
@@ -473,7 +473,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49:J53"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -637,7 +637,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="F8" s="3">
-        <v>570</v>
+        <v>555</v>
       </c>
       <c r="G8">
         <v>1662.6</v>
@@ -733,7 +733,7 @@
         <v>10.4</v>
       </c>
       <c r="F13" s="3">
-        <v>547</v>
+        <v>524</v>
       </c>
       <c r="G13">
         <v>1206.4000000000001</v>
@@ -811,7 +811,7 @@
         <v>10.7</v>
       </c>
       <c r="F17" s="3">
-        <v>588</v>
+        <v>563</v>
       </c>
       <c r="G17">
         <v>952.3</v>

</xml_diff>